<commit_message>
Fix bug, when removing footnote for minute version 4
</commit_message>
<xml_diff>
--- a/data/raw/minutes_format.xlsx
+++ b/data/raw/minutes_format.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MatheusBreitenbach\Documents\VSCode_Projects\0 - TCC\br-central-bank-sentiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MatheusBreitenbach\Documents\VSCode_Projects\0 - TCC\br-central-bank-sentiment\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB34DCA-8A0E-49EB-B28E-796F345D267B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3394FBD-F104-4477-8998-9BFA05C9AC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -747,7 +747,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -767,6 +767,19 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -843,7 +856,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -886,6 +899,8 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1168,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E230"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3868,7 +3883,7 @@
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" s="3" t="s">
+      <c r="A159" s="19" t="s">
         <v>72</v>
       </c>
       <c r="B159" s="11">
@@ -3881,11 +3896,11 @@
         <v>4</v>
       </c>
       <c r="E159" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" s="3" t="s">
+      <c r="A160" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B160" s="11">
@@ -3936,7 +3951,7 @@
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" s="3" t="s">
+      <c r="A163" s="19" t="s">
         <v>68</v>
       </c>
       <c r="B163" s="11">
@@ -3987,7 +4002,7 @@
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" s="3" t="s">
+      <c r="A166" s="18" t="s">
         <v>65</v>
       </c>
       <c r="B166" s="11">
@@ -4004,7 +4019,7 @@
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" s="3" t="s">
+      <c r="A167" s="18" t="s">
         <v>64</v>
       </c>
       <c r="B167" s="11">

</xml_diff>

<commit_message>
Fix bug, breaking paragraghs for minute version 3
</commit_message>
<xml_diff>
--- a/data/raw/minutes_format.xlsx
+++ b/data/raw/minutes_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MatheusBreitenbach\Documents\VSCode_Projects\0 - TCC\br-central-bank-sentiment\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3394FBD-F104-4477-8998-9BFA05C9AC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EFAD88-939D-4768-88D9-5EDF5F546C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -896,11 +896,11 @@
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1184,7 +1184,7 @@
   <dimension ref="A1:E230"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A154" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156"/>
+      <selection activeCell="E166" sqref="A166:E167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,7 +1209,7 @@
       <c r="D1" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="7" t="s">
         <v>233</v>
       </c>
     </row>
@@ -1346,7 +1346,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1363,7 +1363,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1380,7 +1380,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1397,7 +1397,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1414,7 +1414,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1431,7 +1431,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1448,7 +1448,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1465,7 +1465,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1482,7 +1482,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1499,7 +1499,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1516,7 +1516,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1532,7 +1532,7 @@
       <c r="D20" s="9">
         <v>2</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1549,7 +1549,7 @@
       <c r="D21" s="9">
         <v>2</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1566,7 +1566,7 @@
       <c r="D22" s="9">
         <v>2</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1583,7 +1583,7 @@
       <c r="D23" s="9">
         <v>2</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1600,7 +1600,7 @@
       <c r="D24" s="9">
         <v>2</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       <c r="D25" s="9">
         <v>2</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1634,7 +1634,7 @@
       <c r="D26" s="9">
         <v>2</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1651,7 +1651,7 @@
       <c r="D27" s="9">
         <v>2</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1668,8 +1668,8 @@
       <c r="D28" s="9">
         <v>2</v>
       </c>
-      <c r="E28" s="8">
-        <v>0</v>
+      <c r="E28" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1685,7 +1685,7 @@
       <c r="D29" s="9">
         <v>2</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1702,7 +1702,7 @@
       <c r="D30" s="9">
         <v>2</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1719,7 +1719,7 @@
       <c r="D31" s="9">
         <v>2</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1736,7 +1736,7 @@
       <c r="D32" s="9">
         <v>2</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1753,7 +1753,7 @@
       <c r="D33" s="9">
         <v>2</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1770,7 +1770,7 @@
       <c r="D34" s="9">
         <v>2</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1787,7 +1787,7 @@
       <c r="D35" s="9">
         <v>2</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1804,7 +1804,7 @@
       <c r="D36" s="9">
         <v>2</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       <c r="D37" s="9">
         <v>2</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1838,7 +1838,7 @@
       <c r="D38" s="9">
         <v>2</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1846,7 +1846,7 @@
       <c r="A39" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B39" s="18">
         <v>3</v>
       </c>
       <c r="C39" s="10">
@@ -1855,15 +1855,15 @@
       <c r="D39" s="10">
         <v>1</v>
       </c>
-      <c r="E39" s="8">
-        <v>0</v>
+      <c r="E39" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="18">
         <v>3</v>
       </c>
       <c r="C40" s="10">
@@ -1872,15 +1872,15 @@
       <c r="D40" s="10">
         <v>1</v>
       </c>
-      <c r="E40" s="8">
-        <v>0</v>
+      <c r="E40" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B41" s="10">
+      <c r="B41" s="18">
         <v>3</v>
       </c>
       <c r="C41" s="10">
@@ -1889,8 +1889,8 @@
       <c r="D41" s="10">
         <v>1</v>
       </c>
-      <c r="E41" s="8">
-        <v>0</v>
+      <c r="E41" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1906,7 +1906,7 @@
       <c r="D42" s="10">
         <v>1</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E42" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1923,7 +1923,7 @@
       <c r="D43" s="10">
         <v>1</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E43" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1940,7 +1940,7 @@
       <c r="D44" s="10">
         <v>1</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E44" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1957,7 +1957,7 @@
       <c r="D45" s="10">
         <v>1</v>
       </c>
-      <c r="E45" s="8">
+      <c r="E45" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1974,7 +1974,7 @@
       <c r="D46" s="10">
         <v>1</v>
       </c>
-      <c r="E46" s="8">
+      <c r="E46" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       <c r="D47" s="10">
         <v>1</v>
       </c>
-      <c r="E47" s="8">
+      <c r="E47" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2008,7 +2008,7 @@
       <c r="D48" s="10">
         <v>1</v>
       </c>
-      <c r="E48" s="8">
+      <c r="E48" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2025,7 +2025,7 @@
       <c r="D49" s="10">
         <v>1</v>
       </c>
-      <c r="E49" s="8">
+      <c r="E49" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2042,7 +2042,7 @@
       <c r="D50" s="10">
         <v>1</v>
       </c>
-      <c r="E50" s="8">
+      <c r="E50" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2059,7 +2059,7 @@
       <c r="D51" s="10">
         <v>1</v>
       </c>
-      <c r="E51" s="8">
+      <c r="E51" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2076,7 +2076,7 @@
       <c r="D52" s="10">
         <v>1</v>
       </c>
-      <c r="E52" s="8">
+      <c r="E52" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2093,7 +2093,7 @@
       <c r="D53" s="10">
         <v>1</v>
       </c>
-      <c r="E53" s="8">
+      <c r="E53" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2110,7 +2110,7 @@
       <c r="D54" s="10">
         <v>1</v>
       </c>
-      <c r="E54" s="8">
+      <c r="E54" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2127,7 +2127,7 @@
       <c r="D55" s="10">
         <v>1</v>
       </c>
-      <c r="E55" s="8">
+      <c r="E55" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2144,7 +2144,7 @@
       <c r="D56" s="10">
         <v>1</v>
       </c>
-      <c r="E56" s="8">
+      <c r="E56" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2161,7 +2161,7 @@
       <c r="D57" s="10">
         <v>1</v>
       </c>
-      <c r="E57" s="8">
+      <c r="E57" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2178,7 +2178,7 @@
       <c r="D58" s="10">
         <v>1</v>
       </c>
-      <c r="E58" s="8">
+      <c r="E58" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2195,7 +2195,7 @@
       <c r="D59" s="10">
         <v>1</v>
       </c>
-      <c r="E59" s="8">
+      <c r="E59" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2212,7 +2212,7 @@
       <c r="D60" s="10">
         <v>1</v>
       </c>
-      <c r="E60" s="8">
+      <c r="E60" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2229,7 +2229,7 @@
       <c r="D61" s="10">
         <v>1</v>
       </c>
-      <c r="E61" s="8">
+      <c r="E61" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2246,7 +2246,7 @@
       <c r="D62" s="10">
         <v>1</v>
       </c>
-      <c r="E62" s="8">
+      <c r="E62" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2263,7 +2263,7 @@
       <c r="D63" s="10">
         <v>1</v>
       </c>
-      <c r="E63" s="8">
+      <c r="E63" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2280,7 +2280,7 @@
       <c r="D64" s="10">
         <v>1</v>
       </c>
-      <c r="E64" s="8">
+      <c r="E64" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2297,7 +2297,7 @@
       <c r="D65" s="10">
         <v>1</v>
       </c>
-      <c r="E65" s="8">
+      <c r="E65" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2314,7 +2314,7 @@
       <c r="D66" s="10">
         <v>1</v>
       </c>
-      <c r="E66" s="8">
+      <c r="E66" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2331,7 +2331,7 @@
       <c r="D67" s="10">
         <v>1</v>
       </c>
-      <c r="E67" s="8">
+      <c r="E67" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2348,7 +2348,7 @@
       <c r="D68" s="10">
         <v>1</v>
       </c>
-      <c r="E68" s="8">
+      <c r="E68" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       <c r="D69" s="10">
         <v>1</v>
       </c>
-      <c r="E69" s="8">
+      <c r="E69" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2382,7 +2382,7 @@
       <c r="D70" s="10">
         <v>1</v>
       </c>
-      <c r="E70" s="8">
+      <c r="E70" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2399,7 +2399,7 @@
       <c r="D71" s="10">
         <v>1</v>
       </c>
-      <c r="E71" s="8">
+      <c r="E71" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2416,7 +2416,7 @@
       <c r="D72" s="10">
         <v>1</v>
       </c>
-      <c r="E72" s="8">
+      <c r="E72" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2433,7 +2433,7 @@
       <c r="D73" s="10">
         <v>1</v>
       </c>
-      <c r="E73" s="8">
+      <c r="E73" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2450,7 +2450,7 @@
       <c r="D74" s="10">
         <v>1</v>
       </c>
-      <c r="E74" s="8">
+      <c r="E74" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2467,7 +2467,7 @@
       <c r="D75" s="10">
         <v>1</v>
       </c>
-      <c r="E75" s="8">
+      <c r="E75" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2484,7 +2484,7 @@
       <c r="D76" s="10">
         <v>1</v>
       </c>
-      <c r="E76" s="8">
+      <c r="E76" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2501,7 +2501,7 @@
       <c r="D77" s="10">
         <v>1</v>
       </c>
-      <c r="E77" s="8">
+      <c r="E77" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2518,7 +2518,7 @@
       <c r="D78" s="10">
         <v>1</v>
       </c>
-      <c r="E78" s="8">
+      <c r="E78" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2535,7 +2535,7 @@
       <c r="D79" s="10">
         <v>1</v>
       </c>
-      <c r="E79" s="8">
+      <c r="E79" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2552,7 +2552,7 @@
       <c r="D80" s="10">
         <v>1</v>
       </c>
-      <c r="E80" s="8">
+      <c r="E80" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2569,7 +2569,7 @@
       <c r="D81" s="10">
         <v>1</v>
       </c>
-      <c r="E81" s="8">
+      <c r="E81" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2586,7 +2586,7 @@
       <c r="D82" s="10">
         <v>1</v>
       </c>
-      <c r="E82" s="8">
+      <c r="E82" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2603,7 +2603,7 @@
       <c r="D83" s="10">
         <v>1</v>
       </c>
-      <c r="E83" s="8">
+      <c r="E83" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2620,7 +2620,7 @@
       <c r="D84" s="10">
         <v>1</v>
       </c>
-      <c r="E84" s="8">
+      <c r="E84" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       <c r="D85" s="10">
         <v>1</v>
       </c>
-      <c r="E85" s="8">
+      <c r="E85" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2654,7 +2654,7 @@
       <c r="D86" s="10">
         <v>1</v>
       </c>
-      <c r="E86" s="8">
+      <c r="E86" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2671,7 +2671,7 @@
       <c r="D87" s="10">
         <v>1</v>
       </c>
-      <c r="E87" s="8">
+      <c r="E87" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2688,7 +2688,7 @@
       <c r="D88" s="10">
         <v>1</v>
       </c>
-      <c r="E88" s="8">
+      <c r="E88" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2705,7 +2705,7 @@
       <c r="D89" s="10">
         <v>1</v>
       </c>
-      <c r="E89" s="8">
+      <c r="E89" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2722,7 +2722,7 @@
       <c r="D90" s="10">
         <v>1</v>
       </c>
-      <c r="E90" s="8">
+      <c r="E90" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2739,7 +2739,7 @@
       <c r="D91" s="10">
         <v>1</v>
       </c>
-      <c r="E91" s="8">
+      <c r="E91" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2756,7 +2756,7 @@
       <c r="D92" s="10">
         <v>1</v>
       </c>
-      <c r="E92" s="8">
+      <c r="E92" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2773,7 +2773,7 @@
       <c r="D93" s="10">
         <v>1</v>
       </c>
-      <c r="E93" s="8">
+      <c r="E93" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2790,7 +2790,7 @@
       <c r="D94" s="10">
         <v>1</v>
       </c>
-      <c r="E94" s="8">
+      <c r="E94" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2807,7 +2807,7 @@
       <c r="D95" s="10">
         <v>1</v>
       </c>
-      <c r="E95" s="8">
+      <c r="E95" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2824,7 +2824,7 @@
       <c r="D96" s="10">
         <v>1</v>
       </c>
-      <c r="E96" s="8">
+      <c r="E96" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2841,7 +2841,7 @@
       <c r="D97" s="10">
         <v>1</v>
       </c>
-      <c r="E97" s="8">
+      <c r="E97" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2858,7 +2858,7 @@
       <c r="D98" s="10">
         <v>1</v>
       </c>
-      <c r="E98" s="8">
+      <c r="E98" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2875,7 +2875,7 @@
       <c r="D99" s="10">
         <v>1</v>
       </c>
-      <c r="E99" s="8">
+      <c r="E99" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2892,7 +2892,7 @@
       <c r="D100" s="10">
         <v>1</v>
       </c>
-      <c r="E100" s="8">
+      <c r="E100" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2909,7 +2909,7 @@
       <c r="D101" s="10">
         <v>1</v>
       </c>
-      <c r="E101" s="8">
+      <c r="E101" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2926,7 +2926,7 @@
       <c r="D102" s="10">
         <v>1</v>
       </c>
-      <c r="E102" s="8">
+      <c r="E102" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2943,7 +2943,7 @@
       <c r="D103" s="10">
         <v>1</v>
       </c>
-      <c r="E103" s="8">
+      <c r="E103" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2960,7 +2960,7 @@
       <c r="D104" s="10">
         <v>1</v>
       </c>
-      <c r="E104" s="8">
+      <c r="E104" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2977,7 +2977,7 @@
       <c r="D105" s="10">
         <v>1</v>
       </c>
-      <c r="E105" s="8">
+      <c r="E105" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2994,7 +2994,7 @@
       <c r="D106" s="10">
         <v>1</v>
       </c>
-      <c r="E106" s="8">
+      <c r="E106" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3011,7 +3011,7 @@
       <c r="D107" s="10">
         <v>1</v>
       </c>
-      <c r="E107" s="8">
+      <c r="E107" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3028,7 +3028,7 @@
       <c r="D108" s="10">
         <v>1</v>
       </c>
-      <c r="E108" s="8">
+      <c r="E108" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3045,7 +3045,7 @@
       <c r="D109" s="10">
         <v>1</v>
       </c>
-      <c r="E109" s="8">
+      <c r="E109" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3062,7 +3062,7 @@
       <c r="D110" s="10">
         <v>1</v>
       </c>
-      <c r="E110" s="8">
+      <c r="E110" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3079,7 +3079,7 @@
       <c r="D111" s="10">
         <v>1</v>
       </c>
-      <c r="E111" s="8">
+      <c r="E111" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3096,7 +3096,7 @@
       <c r="D112" s="10">
         <v>1</v>
       </c>
-      <c r="E112" s="8">
+      <c r="E112" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3113,7 +3113,7 @@
       <c r="D113" s="10">
         <v>1</v>
       </c>
-      <c r="E113" s="8">
+      <c r="E113" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3130,7 +3130,7 @@
       <c r="D114" s="10">
         <v>1</v>
       </c>
-      <c r="E114" s="8">
+      <c r="E114" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3147,7 +3147,7 @@
       <c r="D115" s="10">
         <v>1</v>
       </c>
-      <c r="E115" s="8">
+      <c r="E115" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3164,7 +3164,7 @@
       <c r="D116" s="10">
         <v>1</v>
       </c>
-      <c r="E116" s="8">
+      <c r="E116" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3181,7 +3181,7 @@
       <c r="D117" s="10">
         <v>1</v>
       </c>
-      <c r="E117" s="8">
+      <c r="E117" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3198,7 +3198,7 @@
       <c r="D118" s="10">
         <v>1</v>
       </c>
-      <c r="E118" s="8">
+      <c r="E118" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3215,7 +3215,7 @@
       <c r="D119" s="10">
         <v>1</v>
       </c>
-      <c r="E119" s="8">
+      <c r="E119" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3232,7 +3232,7 @@
       <c r="D120" s="10">
         <v>1</v>
       </c>
-      <c r="E120" s="8">
+      <c r="E120" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3249,7 +3249,7 @@
       <c r="D121" s="10">
         <v>1</v>
       </c>
-      <c r="E121" s="8">
+      <c r="E121" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3266,7 +3266,7 @@
       <c r="D122" s="10">
         <v>1</v>
       </c>
-      <c r="E122" s="8">
+      <c r="E122" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3283,7 +3283,7 @@
       <c r="D123" s="10">
         <v>1</v>
       </c>
-      <c r="E123" s="8">
+      <c r="E123" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3300,7 +3300,7 @@
       <c r="D124" s="10">
         <v>1</v>
       </c>
-      <c r="E124" s="8">
+      <c r="E124" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3317,7 +3317,7 @@
       <c r="D125" s="10">
         <v>1</v>
       </c>
-      <c r="E125" s="8">
+      <c r="E125" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3334,7 +3334,7 @@
       <c r="D126" s="10">
         <v>1</v>
       </c>
-      <c r="E126" s="8">
+      <c r="E126" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3351,7 +3351,7 @@
       <c r="D127" s="10">
         <v>1</v>
       </c>
-      <c r="E127" s="8">
+      <c r="E127" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3368,7 +3368,7 @@
       <c r="D128" s="10">
         <v>1</v>
       </c>
-      <c r="E128" s="8">
+      <c r="E128" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3385,7 +3385,7 @@
       <c r="D129" s="10">
         <v>1</v>
       </c>
-      <c r="E129" s="8">
+      <c r="E129" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3402,7 +3402,7 @@
       <c r="D130" s="10">
         <v>1</v>
       </c>
-      <c r="E130" s="8">
+      <c r="E130" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3419,7 +3419,7 @@
       <c r="D131" s="10">
         <v>1</v>
       </c>
-      <c r="E131" s="8">
+      <c r="E131" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3436,7 +3436,7 @@
       <c r="D132" s="10">
         <v>1</v>
       </c>
-      <c r="E132" s="8">
+      <c r="E132" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3453,7 +3453,7 @@
       <c r="D133" s="10">
         <v>1</v>
       </c>
-      <c r="E133" s="8">
+      <c r="E133" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3470,7 +3470,7 @@
       <c r="D134" s="10">
         <v>1</v>
       </c>
-      <c r="E134" s="8">
+      <c r="E134" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3487,7 +3487,7 @@
       <c r="D135" s="10">
         <v>1</v>
       </c>
-      <c r="E135" s="8">
+      <c r="E135" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3504,7 +3504,7 @@
       <c r="D136" s="10">
         <v>1</v>
       </c>
-      <c r="E136" s="8">
+      <c r="E136" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3521,7 +3521,7 @@
       <c r="D137" s="10">
         <v>1</v>
       </c>
-      <c r="E137" s="8">
+      <c r="E137" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3538,7 +3538,7 @@
       <c r="D138" s="10">
         <v>1</v>
       </c>
-      <c r="E138" s="8">
+      <c r="E138" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3555,7 +3555,7 @@
       <c r="D139" s="10">
         <v>1</v>
       </c>
-      <c r="E139" s="8">
+      <c r="E139" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3572,7 +3572,7 @@
       <c r="D140" s="10">
         <v>1</v>
       </c>
-      <c r="E140" s="8">
+      <c r="E140" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3589,7 +3589,7 @@
       <c r="D141" s="10">
         <v>1</v>
       </c>
-      <c r="E141" s="8">
+      <c r="E141" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3606,7 +3606,7 @@
       <c r="D142" s="10">
         <v>1</v>
       </c>
-      <c r="E142" s="8">
+      <c r="E142" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3623,7 +3623,7 @@
       <c r="D143" s="10">
         <v>1</v>
       </c>
-      <c r="E143" s="8">
+      <c r="E143" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3640,7 +3640,7 @@
       <c r="D144" s="10">
         <v>1</v>
       </c>
-      <c r="E144" s="8">
+      <c r="E144" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3657,7 +3657,7 @@
       <c r="D145" s="10">
         <v>1</v>
       </c>
-      <c r="E145" s="8">
+      <c r="E145" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3674,7 +3674,7 @@
       <c r="D146" s="10">
         <v>1</v>
       </c>
-      <c r="E146" s="8">
+      <c r="E146" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3691,7 +3691,7 @@
       <c r="D147" s="10">
         <v>1</v>
       </c>
-      <c r="E147" s="8">
+      <c r="E147" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3708,7 +3708,7 @@
       <c r="D148" s="10">
         <v>1</v>
       </c>
-      <c r="E148" s="8">
+      <c r="E148" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3725,7 +3725,7 @@
       <c r="D149" s="10">
         <v>1</v>
       </c>
-      <c r="E149" s="8">
+      <c r="E149" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3742,7 +3742,7 @@
       <c r="D150" s="10">
         <v>1</v>
       </c>
-      <c r="E150" s="8">
+      <c r="E150" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3759,7 +3759,7 @@
       <c r="D151" s="10">
         <v>1</v>
       </c>
-      <c r="E151" s="8">
+      <c r="E151" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3776,7 +3776,7 @@
       <c r="D152" s="10">
         <v>1</v>
       </c>
-      <c r="E152" s="8">
+      <c r="E152" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3793,7 +3793,7 @@
       <c r="D153" s="10">
         <v>1</v>
       </c>
-      <c r="E153" s="8">
+      <c r="E153" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3810,7 +3810,7 @@
       <c r="D154" s="10">
         <v>1</v>
       </c>
-      <c r="E154" s="8">
+      <c r="E154" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3827,7 +3827,7 @@
       <c r="D155" s="10">
         <v>1</v>
       </c>
-      <c r="E155" s="8">
+      <c r="E155" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3844,7 +3844,7 @@
       <c r="D156" s="10">
         <v>1</v>
       </c>
-      <c r="E156" s="8">
+      <c r="E156" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3861,7 +3861,7 @@
       <c r="D157" s="10">
         <v>1</v>
       </c>
-      <c r="E157" s="8">
+      <c r="E157" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3878,12 +3878,12 @@
       <c r="D158" s="10">
         <v>1</v>
       </c>
-      <c r="E158" s="8">
+      <c r="E158" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" s="19" t="s">
+      <c r="A159" s="17" t="s">
         <v>72</v>
       </c>
       <c r="B159" s="11">
@@ -3895,12 +3895,12 @@
       <c r="D159" s="15">
         <v>4</v>
       </c>
-      <c r="E159" s="8">
+      <c r="E159" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" s="18" t="s">
+      <c r="A160" s="19" t="s">
         <v>71</v>
       </c>
       <c r="B160" s="11">
@@ -3912,12 +3912,12 @@
       <c r="D160" s="11">
         <v>3</v>
       </c>
-      <c r="E160" s="8">
-        <v>0</v>
+      <c r="E160" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
+      <c r="A161" s="19" t="s">
         <v>70</v>
       </c>
       <c r="B161" s="11">
@@ -3929,12 +3929,12 @@
       <c r="D161" s="11">
         <v>3</v>
       </c>
-      <c r="E161" s="8">
+      <c r="E161" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="3" t="s">
+      <c r="A162" s="19" t="s">
         <v>69</v>
       </c>
       <c r="B162" s="11">
@@ -3946,7 +3946,7 @@
       <c r="D162" s="11">
         <v>3</v>
       </c>
-      <c r="E162" s="8">
+      <c r="E162" s="11">
         <v>0</v>
       </c>
     </row>
@@ -3963,12 +3963,12 @@
       <c r="D163" s="11">
         <v>3</v>
       </c>
-      <c r="E163" s="8">
+      <c r="E163" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" s="3" t="s">
+      <c r="A164" s="19" t="s">
         <v>67</v>
       </c>
       <c r="B164" s="11">
@@ -3980,12 +3980,12 @@
       <c r="D164" s="11">
         <v>3</v>
       </c>
-      <c r="E164" s="8">
+      <c r="E164" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="3" t="s">
+      <c r="A165" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B165" s="11">
@@ -3997,12 +3997,12 @@
       <c r="D165" s="11">
         <v>3</v>
       </c>
-      <c r="E165" s="8">
+      <c r="E165" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" s="18" t="s">
+      <c r="A166" s="19" t="s">
         <v>65</v>
       </c>
       <c r="B166" s="11">
@@ -4014,12 +4014,12 @@
       <c r="D166" s="11">
         <v>3</v>
       </c>
-      <c r="E166" s="8">
-        <v>0</v>
+      <c r="E166" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" s="18" t="s">
+      <c r="A167" s="19" t="s">
         <v>64</v>
       </c>
       <c r="B167" s="11">
@@ -4031,8 +4031,8 @@
       <c r="D167" s="11">
         <v>3</v>
       </c>
-      <c r="E167" s="8">
-        <v>0</v>
+      <c r="E167" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -4048,7 +4048,7 @@
       <c r="D168" s="11">
         <v>3</v>
       </c>
-      <c r="E168" s="8">
+      <c r="E168" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4065,7 +4065,7 @@
       <c r="D169" s="11">
         <v>3</v>
       </c>
-      <c r="E169" s="8">
+      <c r="E169" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4082,7 +4082,7 @@
       <c r="D170" s="11">
         <v>3</v>
       </c>
-      <c r="E170" s="8">
+      <c r="E170" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4099,7 +4099,7 @@
       <c r="D171" s="11">
         <v>3</v>
       </c>
-      <c r="E171" s="8">
+      <c r="E171" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4116,7 +4116,7 @@
       <c r="D172" s="11">
         <v>3</v>
       </c>
-      <c r="E172" s="8">
+      <c r="E172" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4133,7 +4133,7 @@
       <c r="D173" s="11">
         <v>3</v>
       </c>
-      <c r="E173" s="8">
+      <c r="E173" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4150,7 +4150,7 @@
       <c r="D174" s="11">
         <v>3</v>
       </c>
-      <c r="E174" s="8">
+      <c r="E174" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4167,7 +4167,7 @@
       <c r="D175" s="11">
         <v>3</v>
       </c>
-      <c r="E175" s="8">
+      <c r="E175" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4184,7 +4184,7 @@
       <c r="D176" s="11">
         <v>3</v>
       </c>
-      <c r="E176" s="8">
+      <c r="E176" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4201,7 +4201,7 @@
       <c r="D177" s="11">
         <v>3</v>
       </c>
-      <c r="E177" s="8">
+      <c r="E177" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4218,7 +4218,7 @@
       <c r="D178" s="11">
         <v>3</v>
       </c>
-      <c r="E178" s="8">
+      <c r="E178" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4235,7 +4235,7 @@
       <c r="D179" s="11">
         <v>3</v>
       </c>
-      <c r="E179" s="8">
+      <c r="E179" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4252,7 +4252,7 @@
       <c r="D180" s="11">
         <v>3</v>
       </c>
-      <c r="E180" s="8">
+      <c r="E180" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4269,7 +4269,7 @@
       <c r="D181" s="11">
         <v>3</v>
       </c>
-      <c r="E181" s="8">
+      <c r="E181" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4286,7 +4286,7 @@
       <c r="D182" s="11">
         <v>3</v>
       </c>
-      <c r="E182" s="8">
+      <c r="E182" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4303,7 +4303,7 @@
       <c r="D183" s="11">
         <v>3</v>
       </c>
-      <c r="E183" s="8">
+      <c r="E183" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4320,7 +4320,7 @@
       <c r="D184" s="11">
         <v>3</v>
       </c>
-      <c r="E184" s="8">
+      <c r="E184" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4337,7 +4337,7 @@
       <c r="D185" s="11">
         <v>3</v>
       </c>
-      <c r="E185" s="8">
+      <c r="E185" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4354,7 +4354,7 @@
       <c r="D186" s="11">
         <v>3</v>
       </c>
-      <c r="E186" s="8">
+      <c r="E186" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4371,7 +4371,7 @@
       <c r="D187" s="11">
         <v>3</v>
       </c>
-      <c r="E187" s="8">
+      <c r="E187" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4388,7 +4388,7 @@
       <c r="D188" s="11">
         <v>3</v>
       </c>
-      <c r="E188" s="8">
+      <c r="E188" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4405,7 +4405,7 @@
       <c r="D189" s="11">
         <v>3</v>
       </c>
-      <c r="E189" s="8">
+      <c r="E189" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4422,7 +4422,7 @@
       <c r="D190" s="11">
         <v>3</v>
       </c>
-      <c r="E190" s="8">
+      <c r="E190" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4439,7 +4439,7 @@
       <c r="D191" s="11">
         <v>3</v>
       </c>
-      <c r="E191" s="8">
+      <c r="E191" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4456,7 +4456,7 @@
       <c r="D192" s="12">
         <v>3</v>
       </c>
-      <c r="E192" s="8">
+      <c r="E192" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4473,7 +4473,7 @@
       <c r="D193" s="12">
         <v>3</v>
       </c>
-      <c r="E193" s="8">
+      <c r="E193" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4490,7 +4490,7 @@
       <c r="D194" s="12">
         <v>3</v>
       </c>
-      <c r="E194" s="8">
+      <c r="E194" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4507,7 +4507,7 @@
       <c r="D195" s="12">
         <v>3</v>
       </c>
-      <c r="E195" s="8">
+      <c r="E195" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4524,7 +4524,7 @@
       <c r="D196" s="12">
         <v>3</v>
       </c>
-      <c r="E196" s="8">
+      <c r="E196" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4541,7 +4541,7 @@
       <c r="D197" s="12">
         <v>3</v>
       </c>
-      <c r="E197" s="8">
+      <c r="E197" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4558,7 +4558,7 @@
       <c r="D198" s="12">
         <v>3</v>
       </c>
-      <c r="E198" s="8">
+      <c r="E198" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4575,7 +4575,7 @@
       <c r="D199" s="12">
         <v>3</v>
       </c>
-      <c r="E199" s="8">
+      <c r="E199" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4592,7 +4592,7 @@
       <c r="D200" s="12">
         <v>3</v>
       </c>
-      <c r="E200" s="8">
+      <c r="E200" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4609,7 +4609,7 @@
       <c r="D201" s="12">
         <v>3</v>
       </c>
-      <c r="E201" s="8">
+      <c r="E201" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4626,7 +4626,7 @@
       <c r="D202" s="12">
         <v>3</v>
       </c>
-      <c r="E202" s="8">
+      <c r="E202" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4643,7 +4643,7 @@
       <c r="D203" s="12">
         <v>3</v>
       </c>
-      <c r="E203" s="8">
+      <c r="E203" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4660,7 +4660,7 @@
       <c r="D204" s="12">
         <v>3</v>
       </c>
-      <c r="E204" s="8">
+      <c r="E204" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4677,7 +4677,7 @@
       <c r="D205" s="12">
         <v>3</v>
       </c>
-      <c r="E205" s="8">
+      <c r="E205" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4694,7 +4694,7 @@
       <c r="D206" s="12">
         <v>3</v>
       </c>
-      <c r="E206" s="8">
+      <c r="E206" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4711,7 +4711,7 @@
       <c r="D207" s="12">
         <v>3</v>
       </c>
-      <c r="E207" s="8">
+      <c r="E207" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4728,7 +4728,7 @@
       <c r="D208" s="12">
         <v>3</v>
       </c>
-      <c r="E208" s="8">
+      <c r="E208" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4745,7 +4745,7 @@
       <c r="D209" s="12">
         <v>3</v>
       </c>
-      <c r="E209" s="8">
+      <c r="E209" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4762,7 +4762,7 @@
       <c r="D210" s="12">
         <v>3</v>
       </c>
-      <c r="E210" s="8">
+      <c r="E210" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4779,7 +4779,7 @@
       <c r="D211" s="12">
         <v>3</v>
       </c>
-      <c r="E211" s="8">
+      <c r="E211" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4796,7 +4796,7 @@
       <c r="D212" s="12">
         <v>3</v>
       </c>
-      <c r="E212" s="8">
+      <c r="E212" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4813,7 +4813,7 @@
       <c r="D213" s="12">
         <v>3</v>
       </c>
-      <c r="E213" s="8">
+      <c r="E213" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4830,7 +4830,7 @@
       <c r="D214" s="12">
         <v>3</v>
       </c>
-      <c r="E214" s="8">
+      <c r="E214" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4847,7 +4847,7 @@
       <c r="D215" s="12">
         <v>3</v>
       </c>
-      <c r="E215" s="8">
+      <c r="E215" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4864,7 +4864,7 @@
       <c r="D216" s="12">
         <v>3</v>
       </c>
-      <c r="E216" s="8">
+      <c r="E216" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4881,7 +4881,7 @@
       <c r="D217" s="12">
         <v>3</v>
       </c>
-      <c r="E217" s="8">
+      <c r="E217" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4898,7 +4898,7 @@
       <c r="D218" s="12">
         <v>3</v>
       </c>
-      <c r="E218" s="8">
+      <c r="E218" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4915,7 +4915,7 @@
       <c r="D219" s="12">
         <v>3</v>
       </c>
-      <c r="E219" s="8">
+      <c r="E219" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4932,7 +4932,7 @@
       <c r="D220" s="12">
         <v>3</v>
       </c>
-      <c r="E220" s="8">
+      <c r="E220" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4949,7 +4949,7 @@
       <c r="D221" s="12">
         <v>3</v>
       </c>
-      <c r="E221" s="8">
+      <c r="E221" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4966,7 +4966,7 @@
       <c r="D222" s="12">
         <v>3</v>
       </c>
-      <c r="E222" s="8">
+      <c r="E222" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4983,7 +4983,7 @@
       <c r="D223" s="12">
         <v>3</v>
       </c>
-      <c r="E223" s="8">
+      <c r="E223" s="12">
         <v>0</v>
       </c>
     </row>
@@ -5000,7 +5000,7 @@
       <c r="D224" s="12">
         <v>3</v>
       </c>
-      <c r="E224" s="8">
+      <c r="E224" s="12">
         <v>0</v>
       </c>
     </row>
@@ -5017,7 +5017,7 @@
       <c r="D225" s="12">
         <v>3</v>
       </c>
-      <c r="E225" s="8">
+      <c r="E225" s="12">
         <v>0</v>
       </c>
     </row>
@@ -5034,7 +5034,7 @@
       <c r="D226" s="12">
         <v>3</v>
       </c>
-      <c r="E226" s="8">
+      <c r="E226" s="12">
         <v>0</v>
       </c>
     </row>
@@ -5051,7 +5051,7 @@
       <c r="D227" s="12">
         <v>3</v>
       </c>
-      <c r="E227" s="8">
+      <c r="E227" s="12">
         <v>0</v>
       </c>
     </row>
@@ -5068,7 +5068,7 @@
       <c r="D228" s="12">
         <v>3</v>
       </c>
-      <c r="E228" s="8">
+      <c r="E228" s="12">
         <v>0</v>
       </c>
     </row>
@@ -5085,7 +5085,7 @@
       <c r="D229" s="12">
         <v>3</v>
       </c>
-      <c r="E229" s="8">
+      <c r="E229" s="12">
         <v>0</v>
       </c>
     </row>
@@ -5102,12 +5102,11 @@
       <c r="D230" s="12">
         <v>3</v>
       </c>
-      <c r="E230" s="8">
+      <c r="E230" s="12">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D230" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Manually adjust minutes 40-59 +
</commit_message>
<xml_diff>
--- a/data/raw/minutes_format.xlsx
+++ b/data/raw/minutes_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MatheusBreitenbach\Documents\VSCode_Projects\0 - TCC\br-central-bank-sentiment\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EFAD88-939D-4768-88D9-5EDF5F546C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184AC208-085F-434E-ADB8-CEB32D8ECD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$D$230</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$D$231</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="235">
   <si>
     <t>Titulo</t>
   </si>
@@ -741,6 +741,9 @@
   </si>
   <si>
     <t>Ignore</t>
+  </si>
+  <si>
+    <t>42nd Copom minutes</t>
   </si>
 </sst>
 </file>
@@ -856,7 +859,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -900,7 +903,6 @@
     <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1181,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E230"/>
+  <dimension ref="A1:E231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E166" sqref="A166:E167"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,7 +1217,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="B2" s="8">
         <v>1</v>
@@ -1232,16 +1234,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="B3" s="16">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8">
-        <v>0</v>
-      </c>
-      <c r="D3" s="8">
-        <v>2</v>
+        <v>229</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14">
+        <v>1</v>
+      </c>
+      <c r="D3" s="14">
+        <v>3</v>
       </c>
       <c r="E3" s="8">
         <v>1</v>
@@ -1249,7 +1251,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B4" s="16">
         <v>1</v>
@@ -1266,7 +1268,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B5" s="16">
         <v>1</v>
@@ -1283,7 +1285,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B6" s="16">
         <v>1</v>
@@ -1300,7 +1302,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B7" s="16">
         <v>1</v>
@@ -1317,7 +1319,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B8" s="16">
         <v>1</v>
@@ -1334,9 +1336,9 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="B9" s="8">
+        <v>223</v>
+      </c>
+      <c r="B9" s="16">
         <v>1</v>
       </c>
       <c r="C9" s="8">
@@ -1351,7 +1353,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B10" s="8">
         <v>1</v>
@@ -1368,7 +1370,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B11" s="8">
         <v>1</v>
@@ -1385,7 +1387,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B12" s="8">
         <v>1</v>
@@ -1402,7 +1404,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B13" s="8">
         <v>1</v>
@@ -1419,7 +1421,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B14" s="8">
         <v>1</v>
@@ -1436,7 +1438,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B15" s="8">
         <v>1</v>
@@ -1453,7 +1455,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B16" s="8">
         <v>1</v>
@@ -1470,7 +1472,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B17" s="8">
         <v>1</v>
@@ -1487,7 +1489,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B18" s="8">
         <v>1</v>
@@ -1504,43 +1506,43 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8">
+        <v>2</v>
+      </c>
+      <c r="E19" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="B19" s="8">
-        <v>1</v>
-      </c>
-      <c r="C19" s="8">
-        <v>0</v>
-      </c>
-      <c r="D19" s="8">
-        <v>2</v>
-      </c>
-      <c r="E19" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="B20" s="16">
-        <v>2</v>
-      </c>
-      <c r="C20" s="9">
-        <v>0</v>
-      </c>
-      <c r="D20" s="9">
-        <v>2</v>
-      </c>
-      <c r="E20" s="9">
+      <c r="B20" s="8">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8">
+        <v>0</v>
+      </c>
+      <c r="D20" s="8">
+        <v>2</v>
+      </c>
+      <c r="E20" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="B21" s="9">
+        <v>211</v>
+      </c>
+      <c r="B21" s="16">
         <v>2</v>
       </c>
       <c r="C21" s="9">
@@ -1550,12 +1552,12 @@
         <v>2</v>
       </c>
       <c r="E21" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B22" s="9">
         <v>2</v>
@@ -1572,7 +1574,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B23" s="9">
         <v>2</v>
@@ -1589,7 +1591,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B24" s="9">
         <v>2</v>
@@ -1606,7 +1608,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B25" s="9">
         <v>2</v>
@@ -1623,7 +1625,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B26" s="9">
         <v>2</v>
@@ -1640,7 +1642,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B27" s="9">
         <v>2</v>
@@ -1657,7 +1659,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B28" s="9">
         <v>2</v>
@@ -1669,12 +1671,12 @@
         <v>2</v>
       </c>
       <c r="E28" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B29" s="9">
         <v>2</v>
@@ -1686,12 +1688,12 @@
         <v>2</v>
       </c>
       <c r="E29" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B30" s="9">
         <v>2</v>
@@ -1708,7 +1710,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B31" s="9">
         <v>2</v>
@@ -1725,7 +1727,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B32" s="9">
         <v>2</v>
@@ -1742,7 +1744,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B33" s="9">
         <v>2</v>
@@ -1759,7 +1761,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B34" s="9">
         <v>2</v>
@@ -1776,7 +1778,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B35" s="9">
         <v>2</v>
@@ -1793,7 +1795,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B36" s="9">
         <v>2</v>
@@ -1810,7 +1812,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B37" s="9">
         <v>2</v>
@@ -1827,41 +1829,41 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B38" s="9">
+        <v>2</v>
+      </c>
+      <c r="C38" s="9">
+        <v>0</v>
+      </c>
+      <c r="D38" s="9">
+        <v>2</v>
+      </c>
+      <c r="E38" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B38" s="9">
-        <v>2</v>
-      </c>
-      <c r="C38" s="9">
-        <v>0</v>
-      </c>
-      <c r="D38" s="9">
-        <v>2</v>
-      </c>
-      <c r="E38" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="B39" s="18">
-        <v>3</v>
-      </c>
-      <c r="C39" s="10">
-        <v>0</v>
-      </c>
-      <c r="D39" s="10">
-        <v>1</v>
-      </c>
-      <c r="E39" s="10">
-        <v>1</v>
+      <c r="B39" s="9">
+        <v>2</v>
+      </c>
+      <c r="C39" s="9">
+        <v>0</v>
+      </c>
+      <c r="D39" s="9">
+        <v>2</v>
+      </c>
+      <c r="E39" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B40" s="18">
         <v>3</v>
@@ -1878,7 +1880,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B41" s="18">
         <v>3</v>
@@ -1895,9 +1897,9 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="B42" s="10">
+        <v>190</v>
+      </c>
+      <c r="B42" s="18">
         <v>3</v>
       </c>
       <c r="C42" s="10">
@@ -1907,12 +1909,12 @@
         <v>1</v>
       </c>
       <c r="E42" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B43" s="10">
         <v>3</v>
@@ -1929,7 +1931,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B44" s="10">
         <v>3</v>
@@ -1946,7 +1948,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B45" s="10">
         <v>3</v>
@@ -1963,7 +1965,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B46" s="10">
         <v>3</v>
@@ -1980,7 +1982,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B47" s="10">
         <v>3</v>
@@ -1997,7 +1999,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B48" s="10">
         <v>3</v>
@@ -2014,7 +2016,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B49" s="10">
         <v>3</v>
@@ -2031,7 +2033,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B50" s="10">
         <v>3</v>
@@ -2048,7 +2050,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B51" s="10">
         <v>3</v>
@@ -2065,7 +2067,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B52" s="10">
         <v>3</v>
@@ -2082,7 +2084,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B53" s="10">
         <v>3</v>
@@ -2099,7 +2101,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B54" s="10">
         <v>3</v>
@@ -2116,7 +2118,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B55" s="10">
         <v>3</v>
@@ -2133,7 +2135,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B56" s="10">
         <v>3</v>
@@ -2150,7 +2152,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B57" s="10">
         <v>3</v>
@@ -2167,7 +2169,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B58" s="10">
         <v>3</v>
@@ -2184,7 +2186,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B59" s="10">
         <v>3</v>
@@ -2201,7 +2203,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B60" s="10">
         <v>3</v>
@@ -2218,7 +2220,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B61" s="10">
         <v>3</v>
@@ -2235,7 +2237,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B62" s="10">
         <v>3</v>
@@ -2252,7 +2254,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B63" s="10">
         <v>3</v>
@@ -2269,7 +2271,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B64" s="10">
         <v>3</v>
@@ -2286,7 +2288,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B65" s="10">
         <v>3</v>
@@ -2303,7 +2305,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B66" s="10">
         <v>3</v>
@@ -2320,7 +2322,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B67" s="10">
         <v>3</v>
@@ -2337,7 +2339,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B68" s="10">
         <v>3</v>
@@ -2354,7 +2356,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B69" s="10">
         <v>3</v>
@@ -2371,7 +2373,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B70" s="10">
         <v>3</v>
@@ -2388,7 +2390,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B71" s="10">
         <v>3</v>
@@ -2405,7 +2407,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B72" s="10">
         <v>3</v>
@@ -2422,7 +2424,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B73" s="10">
         <v>3</v>
@@ -2439,7 +2441,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B74" s="10">
         <v>3</v>
@@ -2456,7 +2458,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B75" s="10">
         <v>3</v>
@@ -2473,7 +2475,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B76" s="10">
         <v>3</v>
@@ -2490,7 +2492,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B77" s="10">
         <v>3</v>
@@ -2507,7 +2509,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B78" s="10">
         <v>3</v>
@@ -2524,7 +2526,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B79" s="10">
         <v>3</v>
@@ -2541,7 +2543,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B80" s="10">
         <v>3</v>
@@ -2558,7 +2560,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B81" s="10">
         <v>3</v>
@@ -2575,7 +2577,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B82" s="10">
         <v>3</v>
@@ -2592,7 +2594,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B83" s="10">
         <v>3</v>
@@ -2609,7 +2611,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B84" s="10">
         <v>3</v>
@@ -2626,7 +2628,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B85" s="10">
         <v>3</v>
@@ -2643,7 +2645,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B86" s="10">
         <v>3</v>
@@ -2660,7 +2662,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B87" s="10">
         <v>3</v>
@@ -2677,7 +2679,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B88" s="10">
         <v>3</v>
@@ -2694,7 +2696,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B89" s="10">
         <v>3</v>
@@ -2711,7 +2713,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B90" s="10">
         <v>3</v>
@@ -2728,7 +2730,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B91" s="10">
         <v>3</v>
@@ -2745,7 +2747,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B92" s="10">
         <v>3</v>
@@ -2762,7 +2764,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B93" s="10">
         <v>3</v>
@@ -2779,7 +2781,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B94" s="10">
         <v>3</v>
@@ -2796,7 +2798,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B95" s="10">
         <v>3</v>
@@ -2813,7 +2815,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B96" s="10">
         <v>3</v>
@@ -2830,7 +2832,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B97" s="10">
         <v>3</v>
@@ -2847,7 +2849,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B98" s="10">
         <v>3</v>
@@ -2864,7 +2866,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B99" s="10">
         <v>3</v>
@@ -2881,7 +2883,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B100" s="10">
         <v>3</v>
@@ -2898,7 +2900,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B101" s="10">
         <v>3</v>
@@ -2915,7 +2917,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B102" s="10">
         <v>3</v>
@@ -2932,7 +2934,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B103" s="10">
         <v>3</v>
@@ -2949,7 +2951,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B104" s="10">
         <v>3</v>
@@ -2966,7 +2968,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B105" s="10">
         <v>3</v>
@@ -2983,7 +2985,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B106" s="10">
         <v>3</v>
@@ -3000,7 +3002,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B107" s="10">
         <v>3</v>
@@ -3017,7 +3019,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B108" s="10">
         <v>3</v>
@@ -3034,7 +3036,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B109" s="10">
         <v>3</v>
@@ -3051,7 +3053,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B110" s="10">
         <v>3</v>
@@ -3068,7 +3070,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B111" s="10">
         <v>3</v>
@@ -3085,7 +3087,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B112" s="10">
         <v>3</v>
@@ -3102,7 +3104,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B113" s="10">
         <v>3</v>
@@ -3119,7 +3121,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B114" s="10">
         <v>3</v>
@@ -3136,7 +3138,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B115" s="10">
         <v>3</v>
@@ -3153,7 +3155,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B116" s="10">
         <v>3</v>
@@ -3170,7 +3172,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B117" s="10">
         <v>3</v>
@@ -3187,7 +3189,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B118" s="10">
         <v>3</v>
@@ -3204,7 +3206,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B119" s="10">
         <v>3</v>
@@ -3221,7 +3223,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B120" s="10">
         <v>3</v>
@@ -3238,7 +3240,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B121" s="10">
         <v>3</v>
@@ -3255,7 +3257,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B122" s="10">
         <v>3</v>
@@ -3272,7 +3274,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B123" s="10">
         <v>3</v>
@@ -3289,7 +3291,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B124" s="10">
         <v>3</v>
@@ -3306,7 +3308,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B125" s="10">
         <v>3</v>
@@ -3323,7 +3325,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B126" s="10">
         <v>3</v>
@@ -3340,7 +3342,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B127" s="10">
         <v>3</v>
@@ -3357,7 +3359,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B128" s="10">
         <v>3</v>
@@ -3374,7 +3376,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B129" s="10">
         <v>3</v>
@@ -3391,7 +3393,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B130" s="10">
         <v>3</v>
@@ -3408,7 +3410,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B131" s="10">
         <v>3</v>
@@ -3425,7 +3427,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B132" s="10">
         <v>3</v>
@@ -3442,7 +3444,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B133" s="10">
         <v>3</v>
@@ -3459,7 +3461,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B134" s="10">
         <v>3</v>
@@ -3476,7 +3478,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B135" s="10">
         <v>3</v>
@@ -3493,7 +3495,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B136" s="10">
         <v>3</v>
@@ -3510,7 +3512,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B137" s="10">
         <v>3</v>
@@ -3527,7 +3529,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B138" s="10">
         <v>3</v>
@@ -3544,7 +3546,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B139" s="10">
         <v>3</v>
@@ -3561,7 +3563,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B140" s="10">
         <v>3</v>
@@ -3578,7 +3580,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B141" s="10">
         <v>3</v>
@@ -3595,7 +3597,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B142" s="10">
         <v>3</v>
@@ -3612,7 +3614,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B143" s="10">
         <v>3</v>
@@ -3629,7 +3631,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B144" s="10">
         <v>3</v>
@@ -3646,7 +3648,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B145" s="10">
         <v>3</v>
@@ -3663,7 +3665,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B146" s="10">
         <v>3</v>
@@ -3680,7 +3682,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B147" s="10">
         <v>3</v>
@@ -3697,7 +3699,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B148" s="10">
         <v>3</v>
@@ -3714,7 +3716,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B149" s="10">
         <v>3</v>
@@ -3731,7 +3733,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B150" s="10">
         <v>3</v>
@@ -3748,7 +3750,7 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B151" s="10">
         <v>3</v>
@@ -3765,7 +3767,7 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B152" s="10">
         <v>3</v>
@@ -3782,7 +3784,7 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B153" s="10">
         <v>3</v>
@@ -3799,7 +3801,7 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B154" s="10">
         <v>3</v>
@@ -3816,7 +3818,7 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B155" s="10">
         <v>3</v>
@@ -3833,7 +3835,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B156" s="10">
         <v>3</v>
@@ -3850,7 +3852,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B157" s="10">
         <v>3</v>
@@ -3867,41 +3869,41 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B158" s="10">
+        <v>3</v>
+      </c>
+      <c r="C158" s="10">
+        <v>0</v>
+      </c>
+      <c r="D158" s="10">
+        <v>1</v>
+      </c>
+      <c r="E158" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B158" s="10">
-        <v>3</v>
-      </c>
-      <c r="C158" s="10">
-        <v>0</v>
-      </c>
-      <c r="D158" s="10">
-        <v>1</v>
-      </c>
-      <c r="E158" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" s="17" t="s">
+      <c r="B159" s="10">
+        <v>3</v>
+      </c>
+      <c r="C159" s="10">
+        <v>0</v>
+      </c>
+      <c r="D159" s="10">
+        <v>1</v>
+      </c>
+      <c r="E159" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="17" t="s">
         <v>72</v>
-      </c>
-      <c r="B159" s="11">
-        <v>4</v>
-      </c>
-      <c r="C159" s="11">
-        <v>1</v>
-      </c>
-      <c r="D159" s="15">
-        <v>4</v>
-      </c>
-      <c r="E159" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" s="19" t="s">
-        <v>71</v>
       </c>
       <c r="B160" s="11">
         <v>4</v>
@@ -3909,16 +3911,16 @@
       <c r="C160" s="11">
         <v>1</v>
       </c>
-      <c r="D160" s="11">
-        <v>3</v>
+      <c r="D160" s="15">
+        <v>4</v>
       </c>
       <c r="E160" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" s="19" t="s">
-        <v>70</v>
+      <c r="A161" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="B161" s="11">
         <v>4</v>
@@ -3930,12 +3932,12 @@
         <v>3</v>
       </c>
       <c r="E161" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="19" t="s">
-        <v>69</v>
+      <c r="A162" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="B162" s="11">
         <v>4</v>
@@ -3951,8 +3953,8 @@
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" s="19" t="s">
-        <v>68</v>
+      <c r="A163" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="B163" s="11">
         <v>4</v>
@@ -3968,8 +3970,8 @@
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" s="19" t="s">
-        <v>67</v>
+      <c r="A164" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="B164" s="11">
         <v>4</v>
@@ -3985,8 +3987,8 @@
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="19" t="s">
-        <v>66</v>
+      <c r="A165" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="B165" s="11">
         <v>4</v>
@@ -4002,8 +4004,8 @@
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" s="19" t="s">
-        <v>65</v>
+      <c r="A166" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="B166" s="11">
         <v>4</v>
@@ -4015,12 +4017,12 @@
         <v>3</v>
       </c>
       <c r="E166" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" s="19" t="s">
-        <v>64</v>
+      <c r="A167" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="B167" s="11">
         <v>4</v>
@@ -4037,7 +4039,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B168" s="11">
         <v>4</v>
@@ -4049,12 +4051,12 @@
         <v>3</v>
       </c>
       <c r="E168" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B169" s="11">
         <v>4</v>
@@ -4071,7 +4073,7 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B170" s="11">
         <v>4</v>
@@ -4088,7 +4090,7 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B171" s="11">
         <v>4</v>
@@ -4105,7 +4107,7 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B172" s="11">
         <v>4</v>
@@ -4122,7 +4124,7 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B173" s="11">
         <v>4</v>
@@ -4139,7 +4141,7 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B174" s="11">
         <v>4</v>
@@ -4156,7 +4158,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B175" s="11">
         <v>4</v>
@@ -4173,7 +4175,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B176" s="11">
         <v>4</v>
@@ -4190,7 +4192,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B177" s="11">
         <v>4</v>
@@ -4207,7 +4209,7 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B178" s="11">
         <v>4</v>
@@ -4224,7 +4226,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B179" s="11">
         <v>4</v>
@@ -4241,7 +4243,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B180" s="11">
         <v>4</v>
@@ -4258,7 +4260,7 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B181" s="11">
         <v>4</v>
@@ -4275,7 +4277,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B182" s="11">
         <v>4</v>
@@ -4292,7 +4294,7 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B183" s="11">
         <v>4</v>
@@ -4309,7 +4311,7 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B184" s="11">
         <v>4</v>
@@ -4326,7 +4328,7 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B185" s="11">
         <v>4</v>
@@ -4343,7 +4345,7 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B186" s="11">
         <v>4</v>
@@ -4360,7 +4362,7 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B187" s="11">
         <v>4</v>
@@ -4377,7 +4379,7 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B188" s="11">
         <v>4</v>
@@ -4394,7 +4396,7 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B189" s="11">
         <v>4</v>
@@ -4411,7 +4413,7 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B190" s="11">
         <v>4</v>
@@ -4428,7 +4430,7 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B191" s="11">
         <v>4</v>
@@ -4444,25 +4446,25 @@
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A192" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B192" s="12">
-        <v>5</v>
-      </c>
-      <c r="C192" s="12">
-        <v>1</v>
-      </c>
-      <c r="D192" s="12">
-        <v>3</v>
-      </c>
-      <c r="E192" s="12">
+      <c r="A192" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B192" s="11">
+        <v>4</v>
+      </c>
+      <c r="C192" s="11">
+        <v>1</v>
+      </c>
+      <c r="D192" s="11">
+        <v>3</v>
+      </c>
+      <c r="E192" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B193" s="12">
         <v>5</v>
@@ -4479,7 +4481,7 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B194" s="12">
         <v>5</v>
@@ -4496,7 +4498,7 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B195" s="12">
         <v>5</v>
@@ -4513,7 +4515,7 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B196" s="12">
         <v>5</v>
@@ -4530,7 +4532,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B197" s="12">
         <v>5</v>
@@ -4547,7 +4549,7 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B198" s="12">
         <v>5</v>
@@ -4564,7 +4566,7 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B199" s="12">
         <v>5</v>
@@ -4581,7 +4583,7 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B200" s="12">
         <v>5</v>
@@ -4598,7 +4600,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B201" s="12">
         <v>5</v>
@@ -4615,7 +4617,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B202" s="12">
         <v>5</v>
@@ -4632,7 +4634,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B203" s="12">
         <v>5</v>
@@ -4649,7 +4651,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B204" s="12">
         <v>5</v>
@@ -4666,7 +4668,7 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B205" s="12">
         <v>5</v>
@@ -4683,7 +4685,7 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B206" s="12">
         <v>5</v>
@@ -4700,7 +4702,7 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B207" s="12">
         <v>5</v>
@@ -4717,7 +4719,7 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B208" s="12">
         <v>5</v>
@@ -4734,7 +4736,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B209" s="12">
         <v>5</v>
@@ -4751,7 +4753,7 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B210" s="12">
         <v>5</v>
@@ -4768,7 +4770,7 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B211" s="12">
         <v>5</v>
@@ -4785,7 +4787,7 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B212" s="12">
         <v>5</v>
@@ -4802,7 +4804,7 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B213" s="12">
         <v>5</v>
@@ -4819,7 +4821,7 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B214" s="12">
         <v>5</v>
@@ -4836,7 +4838,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B215" s="12">
         <v>5</v>
@@ -4853,7 +4855,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B216" s="12">
         <v>5</v>
@@ -4870,7 +4872,7 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B217" s="12">
         <v>5</v>
@@ -4887,7 +4889,7 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B218" s="12">
         <v>5</v>
@@ -4904,7 +4906,7 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B219" s="12">
         <v>5</v>
@@ -4921,7 +4923,7 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B220" s="12">
         <v>5</v>
@@ -4938,7 +4940,7 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B221" s="12">
         <v>5</v>
@@ -4955,7 +4957,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B222" s="12">
         <v>5</v>
@@ -4972,7 +4974,7 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B223" s="12">
         <v>5</v>
@@ -4989,7 +4991,7 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B224" s="12">
         <v>5</v>
@@ -5006,7 +5008,7 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B225" s="12">
         <v>5</v>
@@ -5023,7 +5025,7 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B226" s="12">
         <v>5</v>
@@ -5040,7 +5042,7 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B227" s="12">
         <v>5</v>
@@ -5057,7 +5059,7 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B228" s="12">
         <v>5</v>
@@ -5074,7 +5076,7 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B229" s="12">
         <v>5</v>
@@ -5091,7 +5093,7 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B230" s="12">
         <v>5</v>
@@ -5103,6 +5105,23 @@
         <v>3</v>
       </c>
       <c r="E230" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B231" s="12">
+        <v>5</v>
+      </c>
+      <c r="C231" s="12">
+        <v>1</v>
+      </c>
+      <c r="D231" s="12">
+        <v>3</v>
+      </c>
+      <c r="E231" s="12">
         <v>0</v>
       </c>
     </row>

</xml_diff>